<commit_message>
Add mario to contibuters
</commit_message>
<xml_diff>
--- a/Test_suit.xlsx
+++ b/Test_suit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\V2C_Based_ADAS_Project_ITI_GP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D115784-536C-4B9E-9B9F-06A668B692CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DC2447-81C4-4BFD-9D57-CC82A0802DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5E39D012-9333-4EDD-90B6-06E163272A8C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{5E39D012-9333-4EDD-90B6-06E163272A8C}"/>
   </bookViews>
   <sheets>
     <sheet name="Cloud" sheetId="10" r:id="rId1"/>
@@ -831,23 +831,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5CDEF96-B86C-4DF9-9564-3E9A56A238E8}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="104" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="104" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" style="16" customWidth="1"/>
-    <col min="3" max="3" width="43.21875" style="16" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="17" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" style="16" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="18" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="16" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="17" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="16" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="18" customWidth="1"/>
     <col min="7" max="7" width="6" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="16"/>
+    <col min="8" max="16384" width="8.85546875" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
@@ -867,7 +867,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>97</v>
       </c>
@@ -887,47 +887,47 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E3" s="17"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D4" s="16"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D5" s="16"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" s="16"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" s="16"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D8" s="16"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" s="16"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10" s="16"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11" s="16"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="16"/>
     </row>
-    <row r="19" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15"/>
       <c r="D19" s="20"/>
       <c r="F19" s="18"/>
     </row>
-    <row r="24" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="D24" s="20"/>
       <c r="F24" s="18"/>
     </row>
-    <row r="25" spans="1:6" s="19" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" s="19" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15"/>
       <c r="D25" s="20"/>
       <c r="F25" s="18"/>
@@ -942,23 +942,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C8474A9-2491-4C97-BD79-42CEDB3CC1AB}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView zoomScale="104" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="104" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="43.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="7" customWidth="1"/>
     <col min="7" max="7" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -978,7 +978,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>54</v>
       </c>
@@ -998,7 +998,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>55</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>56</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>57</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>58</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>59</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>60</v>
       </c>
@@ -1118,7 +1118,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>61</v>
       </c>
@@ -1138,7 +1138,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>62</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>63</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>64</v>
       </c>
@@ -1198,17 +1198,17 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="D19" s="10"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="24" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="D24" s="10"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:6" s="5" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" s="5" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="D25" s="10"/>
       <c r="F25" s="7"/>
@@ -1227,19 +1227,19 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="7" customWidth="1"/>
     <col min="7" max="7" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>31</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>65</v>
       </c>
@@ -1299,21 +1299,21 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="D19" s="10"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="24" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="D24" s="10"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:6" s="5" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" s="5" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="D25" s="10"/>
       <c r="F25" s="7"/>
@@ -1331,19 +1331,19 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1363,7 +1363,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>19</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>80</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>81</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>82</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>83</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>84</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>85</v>
       </c>
@@ -1560,18 +1560,18 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.21875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1591,7 +1591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -1611,7 +1611,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>15</v>
       </c>
@@ -1648,15 +1648,15 @@
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="F5" s="4"/>
     </row>
-    <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="F10" s="4"/>
     </row>
-    <row r="11" spans="1:6" s="5" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" s="5" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="F11" s="4"/>
     </row>
@@ -1674,18 +1674,18 @@
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
@@ -1725,7 +1725,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>36</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>37</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>39</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>40</v>
       </c>
@@ -1865,19 +1865,19 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="12" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="24" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:6" s="5" customFormat="1" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" s="5" customFormat="1" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="F25" s="7"/>
     </row>

</xml_diff>